<commit_message>
Update Fig 1; add organisation types
</commit_message>
<xml_diff>
--- a/data/processed/2022-central-government-organisations.xlsx
+++ b/data/processed/2022-central-government-organisations.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vstraub/Documents/github-repos/decision-services-index/data/processed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\2-research\3-active-projects\2023-desindex\structural-insights-into-uk-gov\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B3D80A-01A7-2642-B0D3-D402EA1569DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{824D767B-8FC2-7541-806A-FBD7DE9C66BD}"/>
+    <workbookView xWindow="3372" yWindow="1320" windowWidth="27636" windowHeight="16944"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$B$1:$B$58</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="106">
   <si>
     <t>HM Courts &amp; Tribunals Service</t>
   </si>
@@ -318,12 +321,48 @@
   </si>
   <si>
     <t>2022_Agencies_and_public_bodies</t>
+  </si>
+  <si>
+    <t>organisation</t>
+  </si>
+  <si>
+    <t>organisation_type</t>
+  </si>
+  <si>
+    <t>Department of Health and Social</t>
+  </si>
+  <si>
+    <t>Medicines and Healthcare products Regulatory Agency</t>
+  </si>
+  <si>
+    <t>executive_agency</t>
+  </si>
+  <si>
+    <t>ministerial_department</t>
+  </si>
+  <si>
+    <t>public_corporation</t>
+  </si>
+  <si>
+    <t>executive_non_departmental_public_body</t>
+  </si>
+  <si>
+    <t>high_profile_group</t>
+  </si>
+  <si>
+    <t>non_departmental_body</t>
+  </si>
+  <si>
+    <t>special_health_authoriy</t>
+  </si>
+  <si>
+    <t>non_ministerial_department</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -382,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -391,6 +430,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,20 +744,513 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7959E3D-1C92-7B49-9380-26E5F1B4520E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:B58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
+    <col min="2" max="2" width="46.09765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:B58">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ministerial_department"/>
+        <filter val="non_ministerial_department"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="62.33203125" customWidth="1"/>
+    <col min="3" max="3" width="62.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
@@ -731,7 +1264,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -745,7 +1278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -759,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -773,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -787,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -801,7 +1334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -815,7 +1348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -829,7 +1362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -843,7 +1376,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -857,7 +1390,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -871,7 +1404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -885,7 +1418,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>65</v>
       </c>
@@ -896,7 +1429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -907,7 +1440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>66</v>
       </c>
@@ -918,7 +1451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -929,7 +1462,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>27</v>
       </c>
@@ -940,7 +1473,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>4</v>
       </c>
@@ -951,7 +1484,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>67</v>
       </c>
@@ -962,7 +1495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>68</v>
       </c>
@@ -973,7 +1506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>69</v>
       </c>
@@ -984,7 +1517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>70</v>
       </c>
@@ -992,7 +1525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>71</v>
       </c>
@@ -1000,7 +1533,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>72</v>
       </c>
@@ -1008,7 +1541,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>19</v>
       </c>
@@ -1016,172 +1549,172 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" t="s">
         <v>57</v>
       </c>

</xml_diff>